<commit_message>
bulk of Sql Query & Script input type datasource changes
</commit_message>
<xml_diff>
--- a/bkend/reporting/src/test/resources/input/unit/reporting/excelreporter/varying-widths-test.xlsx
+++ b/bkend/reporting/src/test/resources/input/unit/reporting/excelreporter/varying-widths-test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1-5Columns" sheetId="1" state="visible" r:id="rId3"/>
@@ -47,9 +47,6 @@
     <t xml:space="preserve">Sheet1-Row1-Col3</t>
   </si>
   <si>
-    <t xml:space="preserve">Sheet1-Row1-Col4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sheet1-Data1</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t xml:space="preserve">Sheet1-Row2-Col3</t>
   </si>
   <si>
-    <t xml:space="preserve">Sheet1-Row2-Col4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sheet1-Data2</t>
   </si>
   <si>
@@ -77,9 +71,6 @@
     <t xml:space="preserve">Sheet1-Row3-Col3</t>
   </si>
   <si>
-    <t xml:space="preserve">Sheet1-Row3-Col4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sheet1-Data3</t>
   </si>
   <si>
@@ -108,14 +99,24 @@
   </si>
   <si>
     <t xml:space="preserve">Sheet2-Data2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheet2-Row3-ColA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheet2-Row3-ColB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheet2-Data3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -181,12 +182,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -315,16 +320,13 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="16.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -354,45 +356,45 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="n">
+        <v>45777.5397278588</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="2" t="n">
+        <v>45777.5397279977</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="2" t="n">
+        <v>45777.5397280324</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -411,53 +413,58 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1048576"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.5"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>